<commit_message>
Uploading the new navigation files
</commit_message>
<xml_diff>
--- a/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
+++ b/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Google Drive/Documents/University/Courses/2020/ENGSCI 700A&amp;B/GOCPI/data/Inputs/GOCPI OseMOSYS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31943FCE-F9DC-E74C-BC50-ABF1484383F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01A2A40-9AFA-9342-BE73-AD63C8A05525}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
   </bookViews>
@@ -25108,8 +25108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E50F9F-9914-BE4A-ADE8-5916B7A5EEBB}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adjusted error in energy sytems model
</commit_message>
<xml_diff>
--- a/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
+++ b/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Google Drive/Documents/University/Courses/2020/ENGSCI 700A&amp;B/GOCPI/data/Inputs/GOCPI OseMOSYS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DEFC83-C826-6449-B0E7-5274AF1FAC86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA876196-C0F1-024A-BA32-56BEE601FFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
   </bookViews>
@@ -25108,8 +25108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E50F9F-9914-BE4A-ADE8-5916B7A5EEBB}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="140" workbookViewId="0">
-      <selection activeCell="C228" sqref="C228"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
INcluded all set parameter functions
</commit_message>
<xml_diff>
--- a/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
+++ b/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Google Drive/Documents/University/Courses/2020/ENGSCI 700A&amp;B/GOCPI/data/Inputs/GOCPI OseMOSYS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187A91D1-836C-C244-A2D2-1502170D4842}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B0BD21-34B3-7841-A6D6-71677971BC5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -25122,8 +25122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E50F9F-9914-BE4A-ADE8-5916B7A5EEBB}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="159" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Trying to access annualised returns
</commit_message>
<xml_diff>
--- a/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
+++ b/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Google Drive/Documents/University/Courses/2020/ENGSCI 700A&amp;B/GOCPI/data/Inputs/GOCPI OseMOSYS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B0BD21-34B3-7841-A6D6-71677971BC5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A11E6-F0CD-D84C-879D-8038355A48AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -25122,7 +25122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E50F9F-9914-BE4A-ADE8-5916B7A5EEBB}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="159" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Improving writing custom functions to create data
</commit_message>
<xml_diff>
--- a/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
+++ b/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Google Drive/Documents/University/Courses/2020/ENGSCI 700A&amp;B/GOCPI/data/Inputs/GOCPI OseMOSYS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A11E6-F0CD-D84C-879D-8038355A48AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C571436-9C15-3745-9164-155FE84332A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
   </bookViews>
@@ -25122,8 +25122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E50F9F-9914-BE4A-ADE8-5916B7A5EEBB}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28479,7 +28479,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>163</v>
       </c>
@@ -28559,7 +28559,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>163</v>
       </c>

</xml_diff>

<commit_message>
Update the model changes
</commit_message>
<xml_diff>
--- a/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
+++ b/data/Inputs/GOCPI OseMOSYS/GOCPI_OseMOSYS_Structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connor/Google Drive/Documents/University/Courses/2020/ENGSCI 700A&amp;B/GOCPI/data/Inputs/GOCPI OseMOSYS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C571436-9C15-3745-9164-155FE84332A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBF4662-2CFC-F74F-B23D-177083E450A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{8DA962F7-3EC7-1A41-B8DA-1F41AB2AC512}"/>
   </bookViews>
@@ -25122,8 +25122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E50F9F-9914-BE4A-ADE8-5916B7A5EEBB}">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="88" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28479,7 +28479,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>163</v>
       </c>
@@ -28559,7 +28559,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>163</v>
       </c>

</xml_diff>